<commit_message>
Add phone number cleaning function and address function
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laksh\OneDrive\Desktop\Git Clones\Excel-Imports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raif/PycharmProjects/Excel-Imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD3C71C-507B-4F76-86E0-82198D281FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E877AC7-0BC8-3D46-80F0-6491BC905190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -256,9 +256,6 @@
     <t>Jason Dudley</t>
   </si>
   <si>
-    <t>36801 Kevin Harbors Apt. 656, Port Laurenport, MD 59547</t>
-  </si>
-  <si>
     <t>028-612-8297</t>
   </si>
   <si>
@@ -344,6 +341,9 @@
   </si>
   <si>
     <t xml:space="preserve">Not Nice </t>
+  </si>
+  <si>
+    <t>36801 Kevin Harbors Apt. 656, Port Laurenport, MD 59547, USA</t>
   </si>
 </sst>
 </file>
@@ -692,63 +692,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="56.85546875" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" customWidth="1"/>
-    <col min="3" max="3" width="34.7109375" customWidth="1"/>
-    <col min="4" max="4" width="56.7109375" customWidth="1"/>
-    <col min="5" max="5" width="86.42578125" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="56.83203125" customWidth="1"/>
+    <col min="2" max="2" width="37.5" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" customWidth="1"/>
+    <col min="4" max="4" width="56.6640625" customWidth="1"/>
+    <col min="5" max="5" width="86.5" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" t="s">
         <v>84</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F2" t="s">
-        <v>87</v>
-      </c>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -762,14 +762,14 @@
         <v>74</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -783,14 +783,14 @@
         <v>70</v>
       </c>
       <c r="E4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -804,14 +804,14 @@
         <v>66</v>
       </c>
       <c r="E5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -825,14 +825,14 @@
         <v>62</v>
       </c>
       <c r="E6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -846,14 +846,14 @@
         <v>58</v>
       </c>
       <c r="E7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -867,13 +867,13 @@
         <v>54</v>
       </c>
       <c r="E8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -887,13 +887,13 @@
         <v>50</v>
       </c>
       <c r="E9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -907,13 +907,13 @@
         <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -927,13 +927,13 @@
         <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F11" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -947,13 +947,13 @@
         <v>38</v>
       </c>
       <c r="E12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -967,13 +967,13 @@
         <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -987,13 +987,13 @@
         <v>30</v>
       </c>
       <c r="E14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F14" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1007,13 +1007,13 @@
         <v>26</v>
       </c>
       <c r="E15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F15" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1027,13 +1027,13 @@
         <v>22</v>
       </c>
       <c r="E16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F16" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1047,13 +1047,13 @@
         <v>18</v>
       </c>
       <c r="E17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F17" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1067,13 +1067,13 @@
         <v>14</v>
       </c>
       <c r="E18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F18" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1087,13 +1087,13 @@
         <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F19" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1107,13 +1107,13 @@
         <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -1127,10 +1127,10 @@
         <v>2</v>
       </c>
       <c r="E21" t="s">
+        <v>105</v>
+      </c>
+      <c r="F21" t="s">
         <v>106</v>
-      </c>
-      <c r="F21" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>